<commit_message>
feat: adding load and process routes
</commit_message>
<xml_diff>
--- a/data/raw/Bitacora_ELAX.xlsx
+++ b/data/raw/Bitacora_ELAX.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erosj\OneDrive\Escritorio\Multiplica\VitaPro\Repositorios\scope-project\data\raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erosj\OneDrive\Escritorio\Multiplica\VitaPro\Repositorios\scope-fastapi\data\raw\backup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{395615EB-B075-4BAE-8F8F-01927F212717}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84A61706-30E3-4C73-9C84-16697167BD70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="75" yWindow="225" windowWidth="28545" windowHeight="15210" activeTab="1" xr2:uid="{E2D5E726-6FAC-4B5F-A72C-9CA373F62F42}"/>
+    <workbookView xWindow="165" yWindow="195" windowWidth="28545" windowHeight="15210" activeTab="1" xr2:uid="{E2D5E726-6FAC-4B5F-A72C-9CA373F62F42}"/>
   </bookViews>
   <sheets>
     <sheet name="Listas" sheetId="2" r:id="rId1"/>
@@ -4802,10 +4802,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{194842AF-79AC-41D3-AACA-CE5F32DE8343}">
   <dimension ref="A1:AW159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N2" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="L2" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="O2" sqref="O2"/>
-      <selection pane="bottomLeft" activeCell="Q2" sqref="O2:Q2"/>
+      <selection pane="bottomLeft" activeCell="T3" sqref="T3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>